<commit_message>
modifs for exchange reactions
</commit_message>
<xml_diff>
--- a/metabolicReactions.xlsx
+++ b/metabolicReactions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="219">
   <si>
     <t xml:space="preserve">ID (BIGG)</t>
   </si>
@@ -36,6 +36,9 @@
     <t xml:space="preserve">Reaction</t>
   </si>
   <si>
+    <t xml:space="preserve">exchange</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEED link</t>
   </si>
   <si>
@@ -54,6 +57,9 @@
     <t xml:space="preserve">D-Glucose[1] + H+[1] &lt;=&gt; D-Glucose + H+</t>
   </si>
   <si>
+    <t xml:space="preserve">D-Glucose[1]</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://modelseed.org/biochem/reactions/rxn05573</t>
   </si>
   <si>
@@ -283,6 +289,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pyruvate[1] + H+[1] &lt;=&gt; Pyruvate + H+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyruvate[1]</t>
   </si>
   <si>
     <t xml:space="preserve">https://modelseed.org/biochem/reactions/rxn05469</t>
@@ -679,7 +688,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -732,6 +741,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -778,7 +792,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -801,6 +815,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -881,21 +899,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="80.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="76.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="207.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="43.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="207.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -917,427 +935,452 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>77</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>81</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>97</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F22" s="2"/>
+        <v>115</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://modelseed.org/biochem/reactions/rxn00216"/>
+    <hyperlink ref="F3" r:id="rId1" display="https://modelseed.org/biochem/reactions/rxn00216"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1356,8 +1399,8 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1385,402 +1428,402 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1805,7 +1848,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1832,445 +1875,445 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>